<commit_message>
SCRIPT DQL e Documentação
</commit_message>
<xml_diff>
--- a/Banco de Dados/Modelagem/SP-Medical-Group-FÍSICO.xlsx
+++ b/Banco de Dados/Modelagem/SP-Medical-Group-FÍSICO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/480d5ffb018c6fc9/Documentos/SENAI/Projeto_SP_Medical_Group/Banco de Dados/Modelagem/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elilt\OneDrive\Documentos\SENAI\Projeto_SP_Medical_Group\Banco de Dados\Modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8_{63F70432-0D3C-4515-A010-B88A6D64B46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7338FDDA-A16E-4ADF-AE85-8A922E620777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TipoUsuario" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="120" uniqueCount="109">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="109" uniqueCount="98">
   <si>
     <t>idTipoUsuario</t>
   </si>
@@ -242,33 +242,15 @@
     <t>11 3456-7654</t>
   </si>
   <si>
-    <t>43522543-5</t>
-  </si>
-  <si>
     <t>Rua Estado de Israel 240, São Paulo, Estado de São Paulo, 04022-000</t>
   </si>
   <si>
-    <t>7/23/2001</t>
-  </si>
-  <si>
     <t>11 98765-6543</t>
   </si>
   <si>
-    <t>32654345-7</t>
-  </si>
-  <si>
     <t>Av. Paulista, 1578 - Bela Vista, São Paulo - SP, 01310-200</t>
   </si>
   <si>
-    <t>10/13/1985</t>
-  </si>
-  <si>
-    <t>8/27/1975</t>
-  </si>
-  <si>
-    <t>3/21/1972</t>
-  </si>
-  <si>
     <t>11 97208-4453</t>
   </si>
   <si>
@@ -279,21 +261,6 @@
   </si>
   <si>
     <t>11 95436-8769</t>
-  </si>
-  <si>
-    <t>54636525-3</t>
-  </si>
-  <si>
-    <t>54366362-5</t>
-  </si>
-  <si>
-    <t>53254444-1</t>
-  </si>
-  <si>
-    <t>54566266-7</t>
-  </si>
-  <si>
-    <t>54566266-8</t>
   </si>
   <si>
     <t>Av. Ibirapuera - Indianópolis, 2927, São Paulo - SP, 04029-200</t>
@@ -591,7 +558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -678,6 +645,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -961,7 +929,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1062,10 +1030,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1085,10 +1053,10 @@
         <v>22</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1116,10 +1084,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1127,7 +1095,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1135,7 +1103,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1143,7 +1111,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1531,7 +1499,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="E12" s="41">
         <v>404</v>
@@ -1580,7 +1548,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>24</v>
@@ -1653,7 +1621,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,7 +1644,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>62</v>
@@ -1710,14 +1678,14 @@
       <c r="E2" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>68</v>
+      <c r="F2" s="7">
+        <v>435225435</v>
       </c>
       <c r="G2" s="7">
         <v>94839859000</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1730,20 +1698,20 @@
       <c r="C3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>70</v>
+      <c r="D3" s="18" t="d">
+        <v>2001-07-23</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="F3" s="7">
+        <v>326543457</v>
       </c>
       <c r="G3" s="7">
         <v>73556944057</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1760,16 +1728,16 @@
         <v>1978-10-10</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>81</v>
+        <v>71</v>
+      </c>
+      <c r="F4" s="20">
+        <v>546365253</v>
       </c>
       <c r="G4" s="22">
         <v>16839338002</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1782,20 +1750,20 @@
       <c r="C5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>74</v>
+      <c r="D5" s="18" t="d">
+        <v>1985-10-13</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>82</v>
+        <v>72</v>
+      </c>
+      <c r="F5" s="20">
+        <v>543663625</v>
       </c>
       <c r="G5" s="22">
         <v>14332654765</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1808,20 +1776,20 @@
       <c r="C6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="17" t="s">
-        <v>75</v>
+      <c r="D6" s="18" t="d">
+        <v>1975-08-27</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>83</v>
+        <v>73</v>
+      </c>
+      <c r="F6" s="20">
+        <v>532544441</v>
       </c>
       <c r="G6" s="22">
         <v>91305348010</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1834,23 +1802,23 @@
       <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>76</v>
+      <c r="D7" s="18" t="d">
+        <v>1972-03-21</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>84</v>
+        <v>74</v>
+      </c>
+      <c r="F7" s="20">
+        <v>545662667</v>
       </c>
       <c r="G7" s="22">
         <v>79799299004</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1864,14 +1832,14 @@
         <v>2018-05-03</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="21" t="s">
-        <v>85</v>
+      <c r="F8" s="21">
+        <v>545662668</v>
       </c>
       <c r="G8" s="23">
         <v>13771913039</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1883,8 +1851,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9493FE-F5A6-4E59-B1E5-2171F2B21762}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1896,24 +1864,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="9">
         <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1923,10 +1891,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C95DE1B-73F6-4C7F-BBA2-3ACBC1463A4C}">
-  <dimension ref="A4:J18"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D23:D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,165 +1905,166 @@
     <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8">
+        <v>4</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10" t="d">
+        <v>2020-02-01T15:00:00.000</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="42">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2</v>
+      </c>
+      <c r="E3" s="10" t="d">
+        <v>2020-06-01T09:59:59.99999979045242400</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>94</v>
-      </c>
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="42">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10" t="d">
+        <v>2020-07-02T11:00:00.00000020954757600</v>
+      </c>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" s="8">
-        <v>7</v>
-      </c>
-      <c r="C5" s="8">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C5" s="42">
+        <v>3</v>
       </c>
       <c r="D5" s="8">
         <v>1</v>
       </c>
       <c r="E5" s="10" t="d">
-        <v>2020-02-01T15:00:00.000</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>108</v>
-      </c>
+        <v>2018-06-02T09:59:59.99999979045242400</v>
+      </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <v>4</v>
+      </c>
+      <c r="C6" s="42">
         <v>2</v>
-      </c>
-      <c r="B6" s="8">
-        <v>2</v>
-      </c>
-      <c r="C6" s="42">
-        <v>3</v>
       </c>
       <c r="D6" s="8">
         <v>2</v>
       </c>
       <c r="E6" s="10" t="d">
-        <v>2020-06-01T09:59:59.99999979045242400</v>
+        <v>2019-07-02T11:00:00.00000020954757600</v>
       </c>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B7" s="8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C7" s="42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7" s="10" t="d">
-        <v>2020-07-02T11:00:00.00000020954757600</v>
+        <v>2020-08-03T15:00:00.000</v>
       </c>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9">
         <v>4</v>
       </c>
-      <c r="B8" s="8">
+      <c r="C8" s="41">
         <v>2</v>
       </c>
-      <c r="C8" s="42">
-        <v>3</v>
-      </c>
-      <c r="D8" s="8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="10" t="d">
-        <v>2018-06-02T09:59:59.99999979045242400</v>
-      </c>
-      <c r="F8" s="4"/>
+      <c r="D8" s="9">
+        <v>3</v>
+      </c>
+      <c r="E8" s="11" t="d">
+        <v>2020-09-03T11:00:00.00000020954757600</v>
+      </c>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>5</v>
-      </c>
-      <c r="B9" s="8">
-        <v>4</v>
-      </c>
-      <c r="C9" s="42">
-        <v>2</v>
-      </c>
-      <c r="D9" s="8">
-        <v>2</v>
-      </c>
-      <c r="E9" s="10" t="d">
-        <v>2019-07-02T11:00:00.00000020954757600</v>
-      </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>6</v>
-      </c>
-      <c r="B10" s="8">
-        <v>7</v>
-      </c>
-      <c r="C10" s="42">
-        <v>4</v>
-      </c>
-      <c r="D10" s="8">
-        <v>3</v>
-      </c>
-      <c r="E10" s="10" t="d">
-        <v>2020-08-03T15:00:00.000</v>
-      </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
-        <v>7</v>
-      </c>
-      <c r="B11" s="9">
-        <v>4</v>
-      </c>
-      <c r="C11" s="41">
-        <v>2</v>
-      </c>
-      <c r="D11" s="9">
-        <v>3</v>
-      </c>
-      <c r="E11" s="11" t="d">
-        <v>2020-09-03T11:00:00.00000020954757600</v>
-      </c>
-      <c r="F11" s="5"/>
+      <c r="C9" s="43"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="43"/>
+      <c r="J12" s="38"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="38"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J15" s="38"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J16" s="38"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="38"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Página Consultas Adm Completa - Inicialização Projeto React JS
</commit_message>
<xml_diff>
--- a/Banco de Dados/Modelagem/SP-Medical-Group-FÍSICO.xlsx
+++ b/Banco de Dados/Modelagem/SP-Medical-Group-FÍSICO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
   <workbookPr dateCompatibility="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elilt\OneDrive\Documentos\SENAI\Projeto_SP_Medical_Group\Banco de Dados\Modelagem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\45597675800\Documents\SENAI DM\Projeto_SP_Medical_Group\Banco de Dados\Modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7338FDDA-A16E-4ADF-AE85-8A922E620777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5D248C52-24CF-468C-9F3A-CC7CCDD1E3CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TipoUsuario" sheetId="1" r:id="rId1"/>
@@ -933,20 +933,20 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="67.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="67.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -954,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -962,7 +962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -970,7 +970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -979,14 +979,14 @@
       </c>
       <c r="C4" s="38"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H25" s="38"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E50" s="38"/>
     </row>
   </sheetData>
@@ -1003,17 +1003,17 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F11" s="38"/>
     </row>
   </sheetData>
@@ -1076,13 +1076,13 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>81</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F6" s="38"/>
     </row>
   </sheetData>
@@ -1130,13 +1130,13 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1193,7 +1193,7 @@
       </c>
       <c r="E7" s="38"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>11</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>17</v>
       </c>
@@ -1294,14 +1294,14 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="41">
         <v>11</v>
       </c>
@@ -1528,19 +1528,19 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>56</v>
       </c>
@@ -1557,9 +1557,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="32">
         <v>1</v>
@@ -1574,9 +1574,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="12">
         <v>2</v>
@@ -1591,9 +1591,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="13">
         <v>3</v>
@@ -1608,7 +1608,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="38"/>
     </row>
   </sheetData>
@@ -1624,19 +1624,19 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="67.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>61</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1851,18 +1851,18 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9493FE-F5A6-4E59-B1E5-2171F2B21762}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>93</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="41">
         <v>2</v>
       </c>
@@ -1893,19 +1893,19 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C95DE1B-73F6-4C7F-BBA2-3ACBC1463A4C}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>80</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="8">
         <v>1</v>
@@ -1945,7 +1945,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="8">
         <v>2</v>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="8">
         <v>1</v>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="8">
         <v>1</v>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="8">
         <v>2</v>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="8">
         <v>3</v>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="9">
         <v>3</v>
@@ -2053,16 +2053,16 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C9" s="43"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J12" s="38"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J13" s="38"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C15" s="44"/>
       <c r="D15" s="38"/>
     </row>

</xml_diff>